<commit_message>
Split by subjects, evaluation metrics and fancy saving
</commit_message>
<xml_diff>
--- a/EDA/clean_table1.xlsx
+++ b/EDA/clean_table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\PulseOx\mit-sao2-spo2\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B3A281-7CC4-48D9-A8E4-A4B64ABB407B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47466410-491E-4334-9132-64EB4FD1A64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
GridSearch Results; New table one; Inclusion Criteria; Results
</commit_message>
<xml_diff>
--- a/EDA/clean_table1.xlsx
+++ b/EDA/clean_table1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\PulseOx\mit-sao2-spo2\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47466410-491E-4334-9132-64EB4FD1A64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2518C965-54D0-4348-BAF0-E6729621079E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1336,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2866,5 +2866,6 @@
     <mergeCell ref="A14:A18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>